<commit_message>
changed column head name
</commit_message>
<xml_diff>
--- a/debug/testImages/TimeSegments.xlsx
+++ b/debug/testImages/TimeSegments.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenh\Desktop\sr\debug\testImages\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86B5663-33E3-4F52-B8ED-6B219503BF39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="20" windowWidth="20960" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>1080P</t>
   </si>
   <si>
     <t>Group</t>
-  </si>
-  <si>
-    <t>Grab</t>
   </si>
   <si>
     <t>Stitch</t>
@@ -33,13 +44,13 @@
     <t>Broadcast</t>
   </si>
   <si>
-    <t xml:space="preserve">Expected Total Time</t>
+    <t>Expected Total Time</t>
   </si>
   <si>
-    <t xml:space="preserve">Actual Total Time</t>
+    <t>Actual Total Time</t>
   </si>
   <si>
-    <t xml:space="preserve">Wasted Time</t>
+    <t>Wasted Time</t>
   </si>
   <si>
     <t>Above</t>
@@ -83,28 +94,35 @@
   <si>
     <t>4K</t>
   </si>
+  <si>
+    <t>Aggregation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="2"/>
       <name val="Calibri"/>
-      <color indexed="2"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
-    <fill/>
-    <fill/>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -123,20 +141,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -145,16 +166,24 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -166,6 +195,7 @@
       <c:tx>
         <c:rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0">
@@ -178,16 +208,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="en-US"/>
               <a:t>1080p Images Test Time Segments</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
+      <c:spPr>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -196,23 +224,8 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -228,12 +241,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Grab</c:v>
+                  <c:v>Aggregation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -295,46 +308,52 @@
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$14</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="General">
+                <c:pt idx="1">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.3545454545454545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-14E4-4B96-AC94-878F8E79F394}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -350,7 +369,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -412,46 +431,52 @@
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$14</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>2.64696</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>1.60079</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.97034</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="1">
+                  <c:v>1.6007899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97033999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.72102</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>1.25113</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>1.72399</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>1.53299</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="4">
+                  <c:v>1.2511300000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7239899999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5329900000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1.89981</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>3.70769</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>2.01195</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>1.3641</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="8">
+                  <c:v>3.7076899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0119500000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3641000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>1.8573427272727274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-14E4-4B96-AC94-878F8E79F394}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -467,7 +492,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -529,46 +554,52 @@
             <c:numRef>
               <c:f>Sheet1!$D$3:$D$14</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>3.63507</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>3.56692</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>3.57243</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>3.6350699999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5669200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5724300000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>3.61586</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>3.63339</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>3.63738</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="4">
+                  <c:v>3.6158600000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6333899999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6373799999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3.61449</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>3.68509</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>3.65668</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>3.61012</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>3.622743</c:v>
+                <c:pt idx="8">
+                  <c:v>3.6850900000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6566800000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6101200000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6227429999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-14E4-4B96-AC94-878F8E79F394}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -584,7 +615,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -646,46 +677,52 @@
             <c:numRef>
               <c:f>Sheet1!$E$3:$E$14</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0.00544</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.00523</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.00461</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>5.4400000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2300000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6100000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>0.00539</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>0.00693</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.00671</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>0.00449</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>0.00872</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>0.00649</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>0.0046</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>0.005861</c:v>
+                <c:pt idx="4">
+                  <c:v>5.3899999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9300000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7099999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.7200000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8609999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-14E4-4B96-AC94-878F8E79F394}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -696,12 +733,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v xml:space="preserve">Expected Total Time</c:v>
+                  <c:v>Expected Total Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -763,46 +800,52 @@
             <c:numRef>
               <c:f>Sheet1!$F$3:$F$14</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>6.88747</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>5.47294</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>4.847379999999999</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>1.92102</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>5.17238</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>6.8874700000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4729400000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8473799999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9210199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1723800000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5.6643099999999995</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>5.47708</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="6">
+                  <c:v>5.4770799999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5.818789999999999</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>8.0015</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>5.97512</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>5.37882</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>5.51061909090909</c:v>
+                <c:pt idx="8">
+                  <c:v>8.0015000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9751200000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.3788200000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5106190909090902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-14E4-4B96-AC94-878F8E79F394}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -813,12 +856,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v xml:space="preserve">Actual Total Time</c:v>
+                  <c:v>Actual Total Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -880,46 +923,52 @@
             <c:numRef>
               <c:f>Sheet1!$G$3:$G$14</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>30.647</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>29.265</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>30.646999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.265000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>28.593</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>25.684</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="3">
+                  <c:v>25.684000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>29.067</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>29.286</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="5">
+                  <c:v>29.286000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>29.035</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>29.657</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>31.869</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>30.014</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>28.905</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="9">
+                  <c:v>30.013999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.905000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>29.274727272727276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-14E4-4B96-AC94-878F8E79F394}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -930,12 +979,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v xml:space="preserve">Wasted Time</c:v>
+                  <c:v>Wasted Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -997,54 +1046,60 @@
             <c:numRef>
               <c:f>Sheet1!$H$3:$H$14</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>23.759529999999998</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>23.79206</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="1">
+                  <c:v>23.792059999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>23.745620000000002</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>23.762980000000002</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>23.89462</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>23.62169</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>23.55792</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="5">
+                  <c:v>23.621690000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.557919999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>23.83821</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>23.8675</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>24.03888</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="9">
+                  <c:v>24.038879999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>23.52618</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>23.764108181818184</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-14E4-4B96-AC94-878F8E79F394}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-26"/>
@@ -1061,7 +1116,8 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr bwMode="auto">
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
@@ -1077,7 +1133,8 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -1089,7 +1146,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1027"/>
@@ -1107,7 +1164,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -1126,7 +1183,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
+        <c:spPr>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
@@ -1136,7 +1193,8 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -1148,14 +1206,14 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1026"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
+      <c:spPr>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1167,9 +1225,8 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
+      <c:spPr>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1179,7 +1236,8 @@
         </a:ln>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0">
@@ -1191,7 +1249,7 @@
               </a:solidFill>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1199,7 +1257,7 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
+  <c:spPr>
     <a:xfrm>
       <a:off x="2156733" y="5789001"/>
       <a:ext cx="8056996" cy="4549286"/>
@@ -1222,28 +1280,29 @@
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
+    <a:lstStyle/>
     <a:p>
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -1255,6 +1314,7 @@
       <c:tx>
         <c:rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0">
@@ -1267,16 +1327,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr/>
+              <a:rPr lang="en-US"/>
               <a:t>4K Images Test Time Segments</a:t>
             </a:r>
-            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
+      <c:spPr>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1285,23 +1343,8 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1317,12 +1360,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Grab</c:v>
+                  <c:v>Aggregation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -1384,46 +1427,52 @@
             <c:numRef>
               <c:f>Sheet1!$B$17:$B$28</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="General">
+                <c:pt idx="1">
                   <c:v>6.3</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="2">
                   <c:v>6.7</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>6.1</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>6.7</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>8.7</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="7">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>9.718181818181819</c:v>
+                <c:pt idx="11">
+                  <c:v>9.7181818181818187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8151-42AE-8593-D6E9EFEA4374}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1439,7 +1488,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -1501,46 +1550,52 @@
             <c:numRef>
               <c:f>Sheet1!$C$17:$C$28</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>13.69072</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>8.13811</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>5.78881</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>13.690720000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1381099999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7888099999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2.744005</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>6.11946</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>9.72874</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="4">
+                  <c:v>6.1194600000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7287400000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3.58528</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>11.44935</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>18.80005</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="7">
+                  <c:v>11.449350000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.800049999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>11.92863</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>8.40565</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>9.125345909090909</c:v>
+                <c:pt idx="10">
+                  <c:v>8.4056499999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.1253459090909086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8151-42AE-8593-D6E9EFEA4374}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1556,7 +1611,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -1618,46 +1673,52 @@
             <c:numRef>
               <c:f>Sheet1!$D$17:$D$28</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>4.80112</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>4.47609</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>4.40605</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>4.8011200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4760900000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4060499999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>4.37964</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="4">
+                  <c:v>4.3796400000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>4.97797</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>5.00561</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>5.33604</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>5.20224</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>4.73013</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="7">
+                  <c:v>5.0056099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3360399999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.2022399999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.7301299999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>4.812765555555556</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8151-42AE-8593-D6E9EFEA4374}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1673,7 +1734,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -1735,46 +1796,52 @@
             <c:numRef>
               <c:f>Sheet1!$E$17:$E$28</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0.03286</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.03448</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.0303</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>3.286E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4479999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>0.03721</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>0.06081</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="4">
+                  <c:v>3.721E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0810000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>0.03394</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>0.07573</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>0.04906</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>0.03086</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>0.042805555555555555</c:v>
+                <c:pt idx="7">
+                  <c:v>3.3939999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5730000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9059999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0859999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2805555555555555E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8151-42AE-8593-D6E9EFEA4374}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1785,12 +1852,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v xml:space="preserve">Expected Total Time</c:v>
+                  <c:v>Expected Total Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -1852,46 +1919,52 @@
             <c:numRef>
               <c:f>Sheet1!$F$17:$F$28</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>33.524699999999996</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="General">
+                <c:pt idx="1">
                   <c:v>18.948679999999996</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>16.92516</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>8.844005</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="2">
+                  <c:v>16.925160000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.8440049999999992</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>17.236310000000003</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>25.76752</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="5">
+                  <c:v>25.767520000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>12.085280000000001</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>25.1889</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>41.211819999999996</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>28.17993</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="9">
+                  <c:v>28.179929999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>23.06664</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>22.816267727272727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8151-42AE-8593-D6E9EFEA4374}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1902,12 +1975,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v xml:space="preserve">Actual Total Time</c:v>
+                  <c:v>Actual Total Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -1969,46 +2042,52 @@
             <c:numRef>
               <c:f>Sheet1!$G$17:$G$28</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>57.404</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>42.864</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>40.892</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>32.576</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>41.068</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>49.544</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>35.842</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>49.111</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>65.077</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="0">
+                  <c:v>57.404000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.863999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.892000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.576000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.067999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.543999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.841999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49.110999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65.076999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>52.442</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>46.895</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>46.70136363636363</c:v>
+                <c:pt idx="10">
+                  <c:v>46.895000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46.701363636363631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8151-42AE-8593-D6E9EFEA4374}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -2019,12 +2098,12 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v xml:space="preserve">Wasted Time</c:v>
+                  <c:v>Wasted Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -2086,54 +2165,60 @@
             <c:numRef>
               <c:f>Sheet1!$H$17:$H$28</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>23.879300000000008</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>23.91532</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>23.96684</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>23.731995</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="1">
+                  <c:v>23.915320000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.966840000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.731995000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>23.831689999999995</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>23.776479999999996</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>23.756719999999998</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>23.922099999999997</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>23.865180000000002</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>24.26207</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="9">
+                  <c:v>24.262070000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>23.828360000000004</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>23.88509590909091</c:v>
+                <c:pt idx="11">
+                  <c:v>23.885095909090911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8151-42AE-8593-D6E9EFEA4374}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-26"/>
@@ -2150,7 +2235,8 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr bwMode="auto">
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
@@ -2166,7 +2252,8 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -2178,7 +2265,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1034"/>
@@ -2196,7 +2283,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
+          <c:spPr>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -2215,7 +2302,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
+        <c:spPr>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
@@ -2225,7 +2312,8 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0">
@@ -2237,14 +2325,14 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1033"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
+      <c:spPr>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -2256,9 +2344,8 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
+      <c:spPr>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -2268,7 +2355,8 @@
         </a:ln>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="true" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0">
@@ -2280,7 +2368,7 @@
               </a:solidFill>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2288,7 +2376,7 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
+  <c:spPr>
     <a:xfrm>
       <a:off x="2156733" y="10667236"/>
       <a:ext cx="8027688" cy="4843859"/>
@@ -2311,23 +2399,24 @@
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
+    <a:lstStyle/>
     <a:p>
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2341,16 +2430,22 @@
       <xdr:row>56</xdr:row>
       <xdr:rowOff>80596</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="" hidden="0"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2156733" y="5789001"/>
-        <a:ext cx="8056996" cy="4549286"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2373,16 +2468,22 @@
       <xdr:row>84</xdr:row>
       <xdr:rowOff>157528</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="" hidden="0"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2156733" y="10667236"/>
-        <a:ext cx="8027688" cy="4843859"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2395,291 +2496,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2882,779 +2700,782 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="10.7109375"/>
-    <col customWidth="1" min="6" max="6" width="19.421875"/>
-    <col customWidth="1" min="7" max="7" width="22.421875"/>
-    <col customWidth="1" min="8" max="8" width="17.57421875"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="14.25" r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
-    <row ht="14.25" r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.64696</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.6350699999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5.4400000000000004E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F13" si="0">SUM(B3:E3)</f>
+        <v>6.8874700000000004</v>
+      </c>
+      <c r="G3" s="1">
+        <v>30.646999999999998</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H13" si="1">(G3-F3)</f>
+        <v>23.759529999999998</v>
+      </c>
     </row>
-    <row ht="14.25" r="3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.59999999999999998</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2.64696</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3.6350699999999998</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.0054400000000000004</v>
-      </c>
-      <c r="F3" s="2">
-        <f>SUM(B3:E3)</f>
-        <v>6.8874700000000004</v>
-      </c>
-      <c r="G3" s="2">
-        <v>30.646999999999998</v>
-      </c>
-      <c r="H3" s="2">
-        <f>(G3-F3)</f>
-        <v>23.759529999999998</v>
+      <c r="B4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.6007899999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.5669200000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.2300000000000003E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4729400000000004</v>
+      </c>
+      <c r="G4" s="1">
+        <v>29.265000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>23.792059999999999</v>
       </c>
     </row>
-    <row ht="14.25" r="4">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.6007899999999999</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.5669200000000001</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.0052300000000000003</v>
-      </c>
-      <c r="F4" s="2">
-        <f>SUM(B4:E4)</f>
-        <v>5.4729400000000004</v>
-      </c>
-      <c r="G4" s="2">
-        <v>29.265000000000001</v>
-      </c>
-      <c r="H4" s="2">
-        <f>(G4-F4)</f>
-        <v>23.792059999999999</v>
+      <c r="B5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.97033999999999998</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.5724300000000002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.6100000000000004E-3</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8473799999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <v>28.593</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>23.745620000000002</v>
       </c>
     </row>
-    <row ht="14.25" r="5">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.97033999999999998</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3.5724300000000002</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.0046100000000000004</v>
-      </c>
-      <c r="F5" s="2">
-        <f>SUM(B5:E5)</f>
-        <v>4.8473799999999994</v>
-      </c>
-      <c r="G5" s="2">
-        <v>28.593</v>
-      </c>
-      <c r="H5" s="2">
-        <f>(G5-F5)</f>
-        <v>23.745620000000002</v>
+      <c r="B6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.72102</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9210199999999999</v>
+      </c>
+      <c r="G6" s="1">
+        <v>25.684000000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>23.762980000000002</v>
       </c>
     </row>
-    <row ht="14.25" r="6">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.2511300000000001</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.6158600000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.3899999999999998E-3</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1723800000000004</v>
+      </c>
+      <c r="G7" s="1">
+        <v>29.067</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>23.89462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.7239899999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.6333899999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6.9300000000000004E-3</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6643099999999995</v>
+      </c>
+      <c r="G8" s="1">
+        <v>29.286000000000001</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>23.621690000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.5329900000000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.6373799999999998</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.7099999999999998E-3</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4770799999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>29.035</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>23.557919999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.89981</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3.61449</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4.4900000000000001E-3</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.818789999999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>29.657</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>23.83821</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.7076899999999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.6850900000000002</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8.7200000000000003E-3</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>8.0015000000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>31.869</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>23.8675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.0119500000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.6566800000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>6.4900000000000001E-3</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9751200000000004</v>
+      </c>
+      <c r="G12" s="1">
+        <v>30.013999999999999</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>24.038879999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.3641000000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.6101200000000002</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3788200000000002</v>
+      </c>
+      <c r="G13" s="1">
+        <v>28.905000000000001</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>23.52618</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" ref="B14:H14" si="2">AVERAGE(B3:B13)</f>
+        <v>0.3545454545454545</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8573427272727274</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="2"/>
+        <v>3.6227429999999998</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="2"/>
+        <v>5.8609999999999999E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="2"/>
+        <v>5.5106190909090902</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>29.274727272727276</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="2"/>
+        <v>23.764108181818184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <v>13.690720000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4.8011200000000001</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.286E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" ref="F17:F27" si="3">SUM(B17:E17)</f>
+        <v>33.524699999999996</v>
+      </c>
+      <c r="G17" s="1">
+        <v>57.404000000000003</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" ref="H17:H27" si="4">(G17-F17)</f>
+        <v>23.879300000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8.1381099999999993</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4.4760900000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3.4479999999999997E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="3"/>
+        <v>18.948679999999996</v>
+      </c>
+      <c r="G18" s="1">
+        <v>42.863999999999997</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="4"/>
+        <v>23.915320000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5.7888099999999998</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4.4060499999999996</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="3"/>
+        <v>16.925160000000002</v>
+      </c>
+      <c r="G19" s="1">
+        <v>40.892000000000003</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="4"/>
+        <v>23.966840000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2.744005</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.72102</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="3"/>
+        <v>8.8440049999999992</v>
+      </c>
+      <c r="G20" s="1">
+        <v>32.576000000000001</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="4"/>
+        <v>23.731995000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2">
-        <f>SUM(B6:E6)</f>
-        <v>1.9210199999999999</v>
-      </c>
-      <c r="G6" s="2">
-        <v>25.684000000000001</v>
-      </c>
-      <c r="H6" s="2">
-        <f>(G6-F6)</f>
-        <v>23.762980000000002</v>
+      <c r="B21" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6.1194600000000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4.3796400000000002</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3.721E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="3"/>
+        <v>17.236310000000003</v>
+      </c>
+      <c r="G21" s="1">
+        <v>41.067999999999998</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="4"/>
+        <v>23.831689999999995</v>
       </c>
     </row>
-    <row ht="14.25" r="7">
-      <c r="A7" s="2" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.2511300000000001</v>
-      </c>
-      <c r="D7" s="2">
-        <v>3.6158600000000001</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.0053899999999999998</v>
-      </c>
-      <c r="F7" s="2">
-        <f>SUM(B7:E7)</f>
-        <v>5.1723800000000004</v>
-      </c>
-      <c r="G7" s="2">
-        <v>29.067</v>
-      </c>
-      <c r="H7" s="2">
-        <f>(G7-F7)</f>
-        <v>23.89462</v>
+      <c r="B22" s="1">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1">
+        <v>9.7287400000000002</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4.97797</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6.0810000000000003E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="3"/>
+        <v>25.767520000000001</v>
+      </c>
+      <c r="G22" s="1">
+        <v>49.543999999999997</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="4"/>
+        <v>23.776479999999996</v>
       </c>
     </row>
-    <row ht="14.25" r="8">
-      <c r="A8" s="2" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.7239899999999999</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3.6333899999999999</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.0069300000000000004</v>
-      </c>
-      <c r="F8" s="2">
-        <f>SUM(B8:E8)</f>
-        <v>5.6643099999999995</v>
-      </c>
-      <c r="G8" s="2">
-        <v>29.286000000000001</v>
-      </c>
-      <c r="H8" s="2">
-        <f>(G8-F8)</f>
-        <v>23.621690000000001</v>
+      <c r="B23" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.58528</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="3"/>
+        <v>12.085280000000001</v>
+      </c>
+      <c r="G23" s="1">
+        <v>35.841999999999999</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="4"/>
+        <v>23.756719999999998</v>
       </c>
     </row>
-    <row ht="14.25" r="9">
-      <c r="A9" s="2" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.5329900000000001</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3.6373799999999998</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.0067099999999999998</v>
-      </c>
-      <c r="F9" s="2">
-        <f>SUM(B9:E9)</f>
-        <v>5.4770799999999999</v>
-      </c>
-      <c r="G9" s="2">
-        <v>29.035</v>
-      </c>
-      <c r="H9" s="2">
-        <f>(G9-F9)</f>
-        <v>23.557919999999999</v>
+      <c r="B24" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C24" s="1">
+        <v>11.449350000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5.0056099999999999</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3.3939999999999998E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="3"/>
+        <v>25.1889</v>
+      </c>
+      <c r="G24" s="1">
+        <v>49.110999999999997</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="4"/>
+        <v>23.922099999999997</v>
       </c>
     </row>
-    <row ht="14.25" r="10">
-      <c r="A10" s="2" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.89981</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3.61449</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.0044900000000000001</v>
-      </c>
-      <c r="F10" s="2">
-        <f>SUM(B10:E10)</f>
-        <v>5.818789999999999</v>
-      </c>
-      <c r="G10" s="2">
-        <v>29.657</v>
-      </c>
-      <c r="H10" s="2">
-        <f>(G10-F10)</f>
-        <v>23.83821</v>
+      <c r="B25" s="1">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1">
+        <v>18.800049999999999</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5.3360399999999997</v>
+      </c>
+      <c r="E25" s="1">
+        <v>7.5730000000000006E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="3"/>
+        <v>41.211819999999996</v>
+      </c>
+      <c r="G25" s="1">
+        <v>65.076999999999998</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="4"/>
+        <v>23.865180000000002</v>
       </c>
     </row>
-    <row ht="14.25" r="11">
-      <c r="A11" s="2" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.59999999999999998</v>
-      </c>
-      <c r="C11" s="2">
-        <v>3.7076899999999999</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3.6850900000000002</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.0087200000000000003</v>
-      </c>
-      <c r="F11" s="2">
-        <f>SUM(B11:E11)</f>
-        <v>8.0015000000000001</v>
-      </c>
-      <c r="G11" s="2">
-        <v>31.869</v>
-      </c>
-      <c r="H11" s="2">
-        <f>(G11-F11)</f>
-        <v>23.8675</v>
+      <c r="B26" s="1">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1">
+        <v>11.92863</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5.2022399999999998</v>
+      </c>
+      <c r="E26" s="1">
+        <v>4.9059999999999999E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="3"/>
+        <v>28.179929999999999</v>
+      </c>
+      <c r="G26" s="1">
+        <v>52.442</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="4"/>
+        <v>24.262070000000001</v>
       </c>
     </row>
-    <row ht="14.25" r="12">
-      <c r="A12" s="2" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2">
-        <v>0.29999999999999999</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2.0119500000000001</v>
-      </c>
-      <c r="D12" s="2">
-        <v>3.6566800000000002</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.0064900000000000001</v>
-      </c>
-      <c r="F12" s="2">
-        <f>SUM(B12:E12)</f>
-        <v>5.9751200000000004</v>
-      </c>
-      <c r="G12" s="2">
-        <v>30.013999999999999</v>
-      </c>
-      <c r="H12" s="2">
-        <f>(G12-F12)</f>
-        <v>24.038879999999999</v>
+      <c r="B27" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="C27" s="1">
+        <v>8.4056499999999996</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4.7301299999999999</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3.0859999999999999E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="3"/>
+        <v>23.06664</v>
+      </c>
+      <c r="G27" s="1">
+        <v>46.895000000000003</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="4"/>
+        <v>23.828360000000004</v>
       </c>
     </row>
-    <row ht="14.25" r="13">
-      <c r="A13" s="2" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2">
-        <v>0.40000000000000002</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1.3641000000000001</v>
-      </c>
-      <c r="D13" s="2">
-        <v>3.6101200000000002</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.0045999999999999999</v>
-      </c>
-      <c r="F13" s="2">
-        <f>SUM(B13:E13)</f>
-        <v>5.3788200000000002</v>
-      </c>
-      <c r="G13" s="2">
-        <v>28.905000000000001</v>
-      </c>
-      <c r="H13" s="2">
-        <f>(G13-F13)</f>
-        <v>23.52618</v>
-      </c>
-    </row>
-    <row ht="14.25" r="14">
-      <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3">
-        <f>AVERAGE(B3:B13)</f>
-        <v>0.3545454545454545</v>
-      </c>
-      <c r="C14" s="3">
-        <f>AVERAGE(C3:C13)</f>
-        <v>1.8573427272727274</v>
-      </c>
-      <c r="D14" s="3">
-        <f>AVERAGE(D3:D13)</f>
-        <v>3.6227429999999998</v>
-      </c>
-      <c r="E14" s="3">
-        <f>AVERAGE(E3:E13)</f>
-        <v>0.0058609999999999999</v>
-      </c>
-      <c r="F14" s="3">
-        <f>AVERAGE(F3:F13)</f>
-        <v>5.5106190909090902</v>
-      </c>
-      <c r="G14" s="3">
-        <f>AVERAGE(G3:G13)</f>
-        <v>29.274727272727276</v>
-      </c>
-      <c r="H14" s="3">
-        <f>AVERAGE(H3:H13)</f>
-        <v>23.764108181818184</v>
-      </c>
-    </row>
-    <row ht="14.25" r="15">
-      <c r="A15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row ht="14.25" r="16">
-      <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row ht="14.25" r="17">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2">
-        <v>13.690720000000001</v>
-      </c>
-      <c r="D17" s="2">
-        <v>4.8011200000000001</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.03286</v>
-      </c>
-      <c r="F17" s="2">
-        <f>SUM(B17:E17)</f>
-        <v>33.524699999999996</v>
-      </c>
-      <c r="G17" s="2">
-        <v>57.404000000000003</v>
-      </c>
-      <c r="H17" s="2">
-        <f>(G17-F17)</f>
-        <v>23.879300000000008</v>
-      </c>
-    </row>
-    <row ht="14.25" r="18">
-      <c r="A18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2">
-        <v>6.2999999999999998</v>
-      </c>
-      <c r="C18" s="2">
-        <v>8.1381099999999993</v>
-      </c>
-      <c r="D18" s="2">
-        <v>4.4760900000000001</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.034479999999999997</v>
-      </c>
-      <c r="F18" s="2">
-        <f>SUM(B18:E18)</f>
-        <v>18.948679999999996</v>
-      </c>
-      <c r="G18" s="2">
-        <v>42.863999999999997</v>
-      </c>
-      <c r="H18" s="2">
-        <f>(G18-F18)</f>
-        <v>23.915320000000001</v>
-      </c>
-    </row>
-    <row ht="14.25" r="19">
-      <c r="A19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="2">
-        <v>6.7000000000000002</v>
-      </c>
-      <c r="C19" s="2">
-        <v>5.7888099999999998</v>
-      </c>
-      <c r="D19" s="2">
-        <v>4.4060499999999996</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.030300000000000001</v>
-      </c>
-      <c r="F19" s="2">
-        <f>SUM(B19:E19)</f>
-        <v>16.925160000000002</v>
-      </c>
-      <c r="G19" s="2">
-        <v>40.892000000000003</v>
-      </c>
-      <c r="H19" s="2">
-        <f>(G19-F19)</f>
-        <v>23.966840000000001</v>
-      </c>
-    </row>
-    <row ht="14.25" r="20">
-      <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2">
-        <v>6.0999999999999996</v>
-      </c>
-      <c r="C20" s="2">
-        <v>2.744005</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2">
-        <f>SUM(B20:E20)</f>
-        <v>8.8440049999999992</v>
-      </c>
-      <c r="G20" s="2">
-        <v>32.576000000000001</v>
-      </c>
-      <c r="H20" s="2">
-        <f>(G20-F20)</f>
-        <v>23.731995000000001</v>
-      </c>
-    </row>
-    <row ht="14.25" r="21">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2">
-        <v>6.7000000000000002</v>
-      </c>
-      <c r="C21" s="2">
-        <v>6.1194600000000001</v>
-      </c>
-      <c r="D21" s="2">
-        <v>4.3796400000000002</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.03721</v>
-      </c>
-      <c r="F21" s="2">
-        <f>SUM(B21:E21)</f>
-        <v>17.236310000000003</v>
-      </c>
-      <c r="G21" s="2">
-        <v>41.067999999999998</v>
-      </c>
-      <c r="H21" s="2">
-        <f>(G21-F21)</f>
-        <v>23.831689999999995</v>
-      </c>
-    </row>
-    <row ht="14.25" r="22">
-      <c r="A22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="2">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2">
-        <v>9.7287400000000002</v>
-      </c>
-      <c r="D22" s="2">
-        <v>4.97797</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.060810000000000003</v>
-      </c>
-      <c r="F22" s="2">
-        <f>SUM(B22:E22)</f>
-        <v>25.767520000000001</v>
-      </c>
-      <c r="G22" s="2">
-        <v>49.543999999999997</v>
-      </c>
-      <c r="H22" s="2">
-        <f>(G22-F22)</f>
-        <v>23.776479999999996</v>
-      </c>
-    </row>
-    <row ht="14.25" r="23">
-      <c r="A23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="C23" s="2">
-        <v>3.58528</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="2">
-        <f>SUM(B23:E23)</f>
-        <v>12.085280000000001</v>
-      </c>
-      <c r="G23" s="2">
-        <v>35.841999999999999</v>
-      </c>
-      <c r="H23" s="2">
-        <f>(G23-F23)</f>
-        <v>23.756719999999998</v>
-      </c>
-    </row>
-    <row ht="14.25" r="24">
-      <c r="A24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="2">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C24" s="2">
-        <v>11.449350000000001</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5.0056099999999999</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.033939999999999998</v>
-      </c>
-      <c r="F24" s="2">
-        <f>SUM(B24:E24)</f>
-        <v>25.1889</v>
-      </c>
-      <c r="G24" s="2">
-        <v>49.110999999999997</v>
-      </c>
-      <c r="H24" s="2">
-        <f>(G24-F24)</f>
-        <v>23.922099999999997</v>
-      </c>
-    </row>
-    <row ht="14.25" r="25">
-      <c r="A25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="2">
-        <v>17</v>
-      </c>
-      <c r="C25" s="2">
-        <v>18.800049999999999</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5.3360399999999997</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0.075730000000000006</v>
-      </c>
-      <c r="F25" s="2">
-        <f>SUM(B25:E25)</f>
-        <v>41.211819999999996</v>
-      </c>
-      <c r="G25" s="2">
-        <v>65.076999999999998</v>
-      </c>
-      <c r="H25" s="2">
-        <f>(G25-F25)</f>
-        <v>23.865180000000002</v>
-      </c>
-    </row>
-    <row ht="14.25" r="26">
-      <c r="A26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="2">
-        <v>11</v>
-      </c>
-      <c r="C26" s="2">
-        <v>11.92863</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5.2022399999999998</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.049059999999999999</v>
-      </c>
-      <c r="F26" s="2">
-        <f>SUM(B26:E26)</f>
-        <v>28.179929999999999</v>
-      </c>
-      <c r="G26" s="2">
-        <v>52.442</v>
-      </c>
-      <c r="H26" s="2">
-        <f>(G26-F26)</f>
-        <v>24.262070000000001</v>
-      </c>
-    </row>
-    <row ht="14.25" r="27">
-      <c r="A27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="2">
-        <v>9.9000000000000004</v>
-      </c>
-      <c r="C27" s="2">
-        <v>8.4056499999999996</v>
-      </c>
-      <c r="D27" s="2">
-        <v>4.7301299999999999</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0.030859999999999999</v>
-      </c>
-      <c r="F27" s="2">
-        <f>SUM(B27:E27)</f>
-        <v>23.06664</v>
-      </c>
-      <c r="G27" s="2">
-        <v>46.895000000000003</v>
-      </c>
-      <c r="H27" s="2">
-        <f>(G27-F27)</f>
-        <v>23.828360000000004</v>
-      </c>
-    </row>
-    <row ht="14.25" r="28">
-      <c r="A28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="3">
-        <f>AVERAGE(B17:B27)</f>
+      <c r="B28" s="2">
+        <f t="shared" ref="B28:H28" si="5">AVERAGE(B17:B27)</f>
         <v>9.7181818181818187</v>
       </c>
-      <c r="C28" s="3">
-        <f>AVERAGE(C17:C27)</f>
+      <c r="C28" s="2">
+        <f t="shared" si="5"/>
         <v>9.1253459090909086</v>
       </c>
-      <c r="D28" s="3">
-        <f>AVERAGE(D17:D27)</f>
+      <c r="D28" s="2">
+        <f t="shared" si="5"/>
         <v>4.812765555555556</v>
       </c>
-      <c r="E28" s="3">
-        <f>AVERAGE(E17:E27)</f>
-        <v>0.042805555555555555</v>
-      </c>
-      <c r="F28" s="3">
-        <f>AVERAGE(F17:F27)</f>
+      <c r="E28" s="2">
+        <f t="shared" si="5"/>
+        <v>4.2805555555555555E-2</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="5"/>
         <v>22.816267727272727</v>
       </c>
-      <c r="G28" s="3">
-        <f>AVERAGE(G17:G27)</f>
+      <c r="G28" s="2">
+        <f t="shared" si="5"/>
         <v>46.701363636363631</v>
       </c>
-      <c r="H28" s="3">
-        <f>AVERAGE(H17:H27)</f>
+      <c r="H28" s="2">
+        <f t="shared" si="5"/>
         <v>23.885095909090911</v>
       </c>
     </row>
@@ -3663,7 +3484,7 @@
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A15:H15"/>
   </mergeCells>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
+  <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>

</xml_diff>